<commit_message>
Minor update to template
</commit_message>
<xml_diff>
--- a/src/Scripts/Database/MetricsTemplate.xlsx
+++ b/src/Scripts/Database/MetricsTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarkKeene\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\das-payments-V2\src\Scripts\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77EDD7FE-F3E2-4990-8D29-A03177C74C3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD1959C-0FBC-4755-A59C-CEB25C79267B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-5805" windowWidth="29040" windowHeight="15990" xr2:uid="{F6F2B7F4-468F-4B4A-8186-26559F2AB236}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{F6F2B7F4-468F-4B4A-8186-26559F2AB236}"/>
   </bookViews>
   <sheets>
     <sheet name="DAS Payments" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Required Payments made this month</t>
   </si>
@@ -85,9 +87,6 @@
   </si>
   <si>
     <t>HBCP</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -458,7 +457,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -490,7 +489,7 @@
         <v>#REF!</v>
       </c>
       <c r="C2" s="3" t="e">
-        <f>B2/A2</f>
+        <f>A2/B2</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -580,12 +579,13 @@
         <f>G5</f>
         <v>0</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>18</v>
+      <c r="D13" s="3" t="e">
+        <f>B13/B2</f>
+        <v>#REF!</v>
       </c>
       <c r="E13" s="3" t="e">
-        <f>B13/A2</f>
-        <v>#DIV/0!</v>
+        <f>D13</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
@@ -615,15 +615,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020153BB9AD06CE488DB2D0B3295AB5A9" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d418bd2946b32aa9ce18e672ea089e33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9b191e0b-ab79-4414-9ee2-4826aac026ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95d31cff9a2d140cdf1a1ecd54b90156" ns3:_="">
     <xsd:import namespace="9b191e0b-ab79-4414-9ee2-4826aac026ee"/>
@@ -755,6 +746,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -762,14 +762,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F95D9D9-2345-4A14-B5CA-9F1E06E63601}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65B2705C-85A8-4EB1-B45B-B7E812C1A540}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -787,6 +779,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F95D9D9-2345-4A14-B5CA-9F1E06E63601}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D8FF543-4B0C-4924-BCE4-8A51F7F1551C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update to metrics template
</commit_message>
<xml_diff>
--- a/src/Scripts/Database/MetricsTemplate.xlsx
+++ b/src/Scripts/Database/MetricsTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\das-payments-V2\src\Scripts\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarkKeene\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD1959C-0FBC-4755-A59C-CEB25C79267B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C6F585D-6779-409B-9EF2-1A1611B0F549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{F6F2B7F4-468F-4B4A-8186-26559F2AB236}"/>
+    <workbookView xWindow="6804" yWindow="-17388" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAS Payments" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,16 +113,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,18 +143,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,20 +484,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F82D28B-0754-4C22-813F-FE2C789B224E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="30.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.46484375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.53125" customWidth="1"/>
   </cols>
@@ -484,13 +515,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
-      <c r="B2" s="1" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="3" t="e">
         <f>A2/B2</f>
-        <v>#REF!</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D2" s="1">
+        <f>B2-A2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -553,7 +585,7 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
@@ -567,7 +599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -579,28 +611,37 @@
         <f>G5</f>
         <v>0</v>
       </c>
-      <c r="D13" s="3" t="e">
-        <f>B13/B2</f>
-        <v>#REF!</v>
+      <c r="D13" s="5" t="e">
+        <f>1-(D14)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="E13" s="3" t="e">
-        <f>D13</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+        <f>B13/A2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="e">
+      <c r="B14" s="1">
         <f>B2-B13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C14" s="1" t="e">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
         <f>B2-C13-C9</f>
-        <v>#REF!</v>
-      </c>
-    </row>
+        <v>0</v>
+      </c>
+      <c r="D14" s="5" t="e">
+        <f>C14/B2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" s="5" t="e">
+        <f>100%-E13</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="2"/>
     </row>
@@ -747,18 +788,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -780,25 +821,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D8FF543-4B0C-4924-BCE4-8A51F7F1551C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9b191e0b-ab79-4414-9ee2-4826aac026ee"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F95D9D9-2345-4A14-B5CA-9F1E06E63601}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D8FF543-4B0C-4924-BCE4-8A51F7F1551C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9b191e0b-ab79-4414-9ee2-4826aac026ee"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>